<commit_message>
vault backup: 2024-06-10 15:52:25
</commit_message>
<xml_diff>
--- a/practice/excel/Excel Formulas and Functions.xlsx
+++ b/practice/excel/Excel Formulas and Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b09f9559f6a16b6c/YouTube-DESKTOP-8UFBUA3/Tutorials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RhysL\Desktop\water_data_pipeline\practice\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{713ECD65-624D-4F2F-AAA5-462C0452D57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9FAACC-D8AA-441C-9FE4-2E75CDE5C9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11745" yWindow="900" windowWidth="38700" windowHeight="15345" tabRatio="808" firstSheet="1" activeTab="1" xr2:uid="{BDA4A948-540F-4141-95A1-E98575811F66}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" tabRatio="808" firstSheet="1" activeTab="4" xr2:uid="{BDA4A948-540F-4141-95A1-E98575811F66}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula Fundamentals" sheetId="12" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="Date &amp; Time" sheetId="10" r:id="rId9"/>
     <sheet name="Bonus" sheetId="11" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="taxrate">'Tax Rate'!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -270,7 +273,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,9 +351,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -388,7 +391,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -494,7 +497,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -636,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,11 +649,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFB1C96-D47E-41A2-BFA9-F360F0CDD5B5}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="122" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -659,7 +662,7 @@
     <col min="6" max="6" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -676,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -689,11 +692,15 @@
       <c r="D2">
         <v>5</v>
       </c>
+      <c r="E2">
+        <f>B2+C2+D2</f>
+        <v>23</v>
+      </c>
       <c r="G2" s="3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -706,42 +713,82 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="E3">
+        <f>B3+C3+D3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="B4">
+        <f>B2-B3</f>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:E4" si="0">C2-C3</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="B5">
+        <f>B4*taxrate</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="C5">
+        <f>C4*taxrate</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <f>D4*taxrate</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E5">
+        <f>E4*taxrate</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B9">
+        <f>E4/2</f>
+        <v>7</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
@@ -754,11 +801,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC952244-2217-4A67-90AC-AD0F61C3E987}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="325" zoomScaleNormal="325" workbookViewId="0"/>
+    <sheetView zoomScale="239" zoomScaleNormal="325" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>5+4</f>
         <v>9</v>
@@ -767,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>8-2</f>
         <v>6</v>
@@ -776,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+B2</f>
         <v>9</v>
@@ -786,7 +833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -804,18 +851,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3504990-CFAE-4B46-98D6-DE9ED6EA08FF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.1</v>
       </c>
@@ -830,15 +877,15 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,7 +893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -857,7 +904,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -865,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -874,22 +921,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B5">
+        <f>B4*D2</f>
+        <v>0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -901,11 +952,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BE7816-1F13-4EB2-B1BF-D99034D19386}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -914,7 +967,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -922,7 +975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -932,8 +985,12 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <f>SUM(B2:B8)</f>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -944,7 +1001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -955,7 +1012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -965,8 +1022,12 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <f>LARGE(B2:B8,2)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -977,7 +1038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -988,7 +1049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -996,17 +1057,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>27</v>
       </c>
@@ -1024,9 +1085,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B872CB-F967-45A8-83C0-EF5A4DD6E9C5}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1034,7 +1095,7 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1045,7 +1106,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1145,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1095,7 +1156,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1120,7 +1181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1162,7 +1223,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1176,7 +1237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1190,7 +1251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1201,7 +1262,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1212,7 +1273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1223,7 +1284,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1234,7 +1295,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1306,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1317,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1267,7 +1328,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1278,7 +1339,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1289,7 +1350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1312,37 +1373,37 @@
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1353,12 +1414,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1369,12 +1430,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1385,37 +1446,37 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
@@ -1435,18 +1496,18 @@
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1454,7 +1515,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1462,15 +1523,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1481,7 +1542,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1500,7 +1561,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1508,27 +1569,27 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
@@ -1539,7 +1600,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1553,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1561,7 +1622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1581,7 +1642,7 @@
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
@@ -1589,7 +1650,7 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -1604,7 +1665,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1621,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1643,12 +1704,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>68</v>
       </c>
@@ -1667,25 +1728,25 @@
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2024-06-10 20:19:16
</commit_message>
<xml_diff>
--- a/practice/excel/Excel Formulas and Functions.xlsx
+++ b/practice/excel/Excel Formulas and Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RhysL\Desktop\water_data_pipeline\practice\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9FAACC-D8AA-441C-9FE4-2E75CDE5C9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74829B7-14D3-4A53-B704-24FC99940FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" tabRatio="808" firstSheet="1" activeTab="4" xr2:uid="{BDA4A948-540F-4141-95A1-E98575811F66}"/>
+    <workbookView xWindow="28680" yWindow="-1245" windowWidth="29040" windowHeight="15720" tabRatio="808" firstSheet="1" activeTab="9" xr2:uid="{BDA4A948-540F-4141-95A1-E98575811F66}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula Fundamentals" sheetId="12" r:id="rId1"/>
@@ -319,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -332,6 +332,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -799,9 +801,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC952244-2217-4A67-90AC-AD0F61C3E987}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="239" zoomScaleNormal="325" workbookViewId="0"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G4" sqref="G2:G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -841,6 +845,12 @@
         <f>B3+A3</f>
         <v>15</v>
       </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1085,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B872CB-F967-45A8-83C0-EF5A4DD6E9C5}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1638,9 +1648,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DF037D-F900-45F8-A4CC-790EE9DB30C3}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F17" sqref="E16:F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1692,6 +1704,10 @@
       <c r="C3">
         <v>3</v>
       </c>
+      <c r="E3">
+        <f>VLOOKUP(F2,A2:C4,2,FALSE)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1715,6 +1731,12 @@
       </c>
       <c r="F6" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>_xlfn.XLOOKUP(F6,A:A,B:B)</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1726,7 +1748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47EA0745-0719-4EE6-B49F-FDC6A9926567}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1739,7 +1763,10 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="6">
+        <f ca="1">TODAY()</f>
+        <v>45453</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">

</xml_diff>